<commit_message>
Move touch 2 mm right
</commit_message>
<xml_diff>
--- a/S3-silicon-Sharp-Touch/fabrication/BOMs.xlsx
+++ b/S3-silicon-Sharp-Touch/fabrication/BOMs.xlsx
@@ -200,7 +200,7 @@
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C5457064</t>
+    <t xml:space="preserve">C525331</t>
   </si>
   <si>
     <t xml:space="preserve">Q3</t>
@@ -414,11 +414,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -455,6 +456,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -499,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,6 +522,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -768,7 +781,7 @@
       <c r="C16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1055,7 +1068,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="atEnd" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>